<commit_message>
Added scaling calculations to xl file
</commit_message>
<xml_diff>
--- a/segmentVolumesDensities.xlsx
+++ b/segmentVolumesDensities.xlsx
@@ -1,22 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26230"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Laura Porro\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chrisrichards/Desktop/FrogWork/Chris/CODE/MuJoCo/mjMOD_3SegRMdevel/RMsim/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="6780"/>
+    <workbookView xWindow="940" yWindow="1020" windowWidth="26620" windowHeight="11640"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
   <si>
     <t>Body segment</t>
   </si>
@@ -66,6 +69,78 @@
   </si>
   <si>
     <t>Foot soft tissues</t>
+  </si>
+  <si>
+    <t>lumped segment mass (from uCT)</t>
+  </si>
+  <si>
+    <t>Body soft tissues</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Pelvic soft tissues</t>
+  </si>
+  <si>
+    <t>segment</t>
+  </si>
+  <si>
+    <t>Body</t>
+  </si>
+  <si>
+    <t>pelvis</t>
+  </si>
+  <si>
+    <t>thigh</t>
+  </si>
+  <si>
+    <t>shank</t>
+  </si>
+  <si>
+    <t>tarsus</t>
+  </si>
+  <si>
+    <t>foot</t>
+  </si>
+  <si>
+    <t>volume weighting (estimated at 0.05 for body and pelvis for now)</t>
+  </si>
+  <si>
+    <t>density weighted avg</t>
+  </si>
+  <si>
+    <t>avg density</t>
+  </si>
+  <si>
+    <t>scaled masses</t>
+  </si>
+  <si>
+    <t>Ratio</t>
+  </si>
+  <si>
+    <t>length</t>
+  </si>
+  <si>
+    <t>length scaled</t>
+  </si>
+  <si>
+    <t>mass 1</t>
+  </si>
+  <si>
+    <t>mass2</t>
+  </si>
+  <si>
+    <t>length 1</t>
+  </si>
+  <si>
+    <t>length 2</t>
+  </si>
+  <si>
+    <t>Nominal mass (g)</t>
+  </si>
+  <si>
+    <t>mass for scaled model (g)</t>
   </si>
 </sst>
 </file>
@@ -81,12 +156,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -101,8 +188,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -383,150 +472,447 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" customWidth="1"/>
+    <col min="2" max="2" width="16.5" customWidth="1"/>
+    <col min="3" max="3" width="18.83203125" customWidth="1"/>
+    <col min="4" max="4" width="30.1640625" customWidth="1"/>
+    <col min="5" max="6" width="18.83203125" customWidth="1"/>
+    <col min="7" max="8" width="26.83203125" customWidth="1"/>
+    <col min="9" max="9" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="1">
+        <v>11.4</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="2">
+        <v>11.4</v>
+      </c>
+      <c r="E2">
+        <f>D2/B2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="D3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B2">
+      <c r="B4">
         <v>260.7</v>
       </c>
-      <c r="C2">
+      <c r="C4">
         <v>1.93</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="D4">
+        <v>0.05</v>
+      </c>
+      <c r="E4">
+        <f>(D4*C4+D5*C5)</f>
+        <v>1.0997000000000001</v>
+      </c>
+      <c r="F4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4">
+        <v>7.1999999999999998E-3</v>
+      </c>
+      <c r="H4">
+        <f>G4*$E$2</f>
+        <v>7.1999999999999998E-3</v>
+      </c>
+      <c r="I4">
+        <f>E4</f>
+        <v>1.0997000000000001</v>
+      </c>
+      <c r="J4">
+        <v>1.9743900000000002E-2</v>
+      </c>
+      <c r="K4">
+        <f>J4*($E$2^(1/3))</f>
+        <v>1.9743900000000002E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5">
+        <v>1.056</v>
+      </c>
+      <c r="D5">
+        <f>1-D4</f>
+        <v>0.95</v>
+      </c>
+      <c r="F5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5">
+        <v>1.2999999999999999E-3</v>
+      </c>
+      <c r="H5">
+        <f t="shared" ref="H5:H9" si="0">G5*$E$2</f>
+        <v>1.2999999999999999E-3</v>
+      </c>
+      <c r="I5">
+        <f>E6</f>
+        <v>1.0997000000000001</v>
+      </c>
+      <c r="J5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>3</v>
       </c>
-      <c r="B3">
+      <c r="B6">
         <v>67.8</v>
       </c>
-      <c r="C3">
+      <c r="C6">
         <v>1.93</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4">
-        <v>7779.7</v>
-      </c>
-      <c r="C4">
+      <c r="D6">
+        <v>0.05</v>
+      </c>
+      <c r="E6">
+        <f>D6*C6+D7*C7</f>
+        <v>1.0997000000000001</v>
+      </c>
+      <c r="F6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6">
+        <v>7.7612999999999998E-4</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>7.7612999999999998E-4</v>
+      </c>
+      <c r="I6">
+        <f>E8</f>
+        <v>1.0806231520223153</v>
+      </c>
+      <c r="J6">
+        <v>1.77912E-2</v>
+      </c>
+      <c r="K6">
+        <f t="shared" ref="K5:K9" si="1">J6*($E$2^(1/3))</f>
+        <v>1.77912E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7">
         <v>1.056</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="D7">
+        <f>1-D6</f>
+        <v>0.95</v>
+      </c>
+      <c r="F7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7">
+        <v>3.6152999999999999E-4</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>3.6152999999999999E-4</v>
+      </c>
+      <c r="I7">
+        <f>E10</f>
+        <v>1.1300727394060728</v>
+      </c>
+      <c r="J7">
+        <v>8.0277000000000005E-3</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="1"/>
+        <v>8.0277000000000005E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B5">
+      <c r="B8">
         <v>20.2</v>
       </c>
-      <c r="C5">
+      <c r="C8">
         <v>1.93</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="D8">
+        <f>B8/B9</f>
+        <v>2.817294281729428E-2</v>
+      </c>
+      <c r="E8">
+        <f>D8*C8+D9*C9</f>
+        <v>1.0806231520223153</v>
+      </c>
+      <c r="F8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8">
+        <v>1.5557E-4</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>1.5557E-4</v>
+      </c>
+      <c r="I8">
+        <f>E12</f>
+        <v>1.154644041041831</v>
+      </c>
+      <c r="J8">
+        <v>8.0277000000000005E-3</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="1"/>
+        <v>8.0277000000000005E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B6">
+      <c r="B9">
         <v>717</v>
       </c>
-      <c r="C6">
+      <c r="C9">
         <v>1.056</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="D9">
+        <f>1-D8</f>
+        <v>0.97182705718270568</v>
+      </c>
+      <c r="F9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9">
+        <v>1.6291999999999999E-4</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>1.6291999999999999E-4</v>
+      </c>
+      <c r="I9">
+        <f>E14</f>
+        <v>1.2015483346872462</v>
+      </c>
+      <c r="J9">
+        <v>0.01</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="1"/>
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>8</v>
       </c>
-      <c r="B7">
+      <c r="B10">
         <v>25.4</v>
       </c>
-      <c r="C7">
+      <c r="C10">
         <v>1.93</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="D10">
+        <f>B10/B11</f>
+        <v>8.4751418084751423E-2</v>
+      </c>
+      <c r="E10">
+        <f>D10*C10+D11*C11</f>
+        <v>1.1300727394060728</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>9</v>
       </c>
-      <c r="B8">
+      <c r="B11">
         <v>299.7</v>
       </c>
-      <c r="C8">
+      <c r="C11">
         <v>1.056</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="D11">
+        <f>1-D10</f>
+        <v>0.9152485819152486</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>10</v>
       </c>
-      <c r="B9">
+      <c r="B12">
         <f>8.8+5.5</f>
         <v>14.3</v>
       </c>
-      <c r="C9">
+      <c r="C12">
         <v>1.93</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="D12">
+        <f>B12/B13</f>
+        <v>0.11286503551696922</v>
+      </c>
+      <c r="E12">
+        <f>D12*C12+D13*C13</f>
+        <v>1.154644041041831</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>11</v>
       </c>
-      <c r="B10">
+      <c r="B13">
         <v>126.7</v>
       </c>
-      <c r="C10">
+      <c r="C13">
         <v>1.056</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="D13">
+        <f>1-D12</f>
+        <v>0.88713496448303075</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>12</v>
       </c>
-      <c r="B11">
+      <c r="B14">
         <f>12.5+4.9+2.4+0.7</f>
         <v>20.499999999999996</v>
       </c>
-      <c r="C11">
+      <c r="C14">
         <v>1.93</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="D14">
+        <f>B14/B15</f>
+        <v>0.16653127538586512</v>
+      </c>
+      <c r="E14">
+        <f>D14*C14+D15*C15</f>
+        <v>1.2015483346872462</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>13</v>
       </c>
-      <c r="B12">
+      <c r="B15">
         <v>123.1</v>
       </c>
-      <c r="C12">
+      <c r="C15">
+        <v>1.056</v>
+      </c>
+      <c r="D15">
+        <f>1-D14</f>
+        <v>0.8334687246141349</v>
+      </c>
+      <c r="G15" t="s">
+        <v>32</v>
+      </c>
+      <c r="H15" t="s">
+        <v>33</v>
+      </c>
+      <c r="I15" t="s">
+        <v>34</v>
+      </c>
+      <c r="J15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G16">
+        <v>27</v>
+      </c>
+      <c r="H16">
+        <v>10</v>
+      </c>
+      <c r="I16">
+        <f>G16^(1/3)</f>
+        <v>2.9999999999999996</v>
+      </c>
+      <c r="J16">
+        <f>I16*(H16/G16)^(1/3)</f>
+        <v>2.1544346900318834</v>
+      </c>
+      <c r="K16">
+        <f>J16^3</f>
+        <v>9.9999999999999947</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18">
+        <v>7779.7</v>
+      </c>
+      <c r="C18">
         <v>1.056</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adding LV code and template file for scaling the model
</commit_message>
<xml_diff>
--- a/segmentVolumesDensities.xlsx
+++ b/segmentVolumesDensities.xlsx
@@ -1,21 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26230"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chrisrichards/Desktop/FrogWork/Chris/CODE/MuJoCo/mjMOD_3SegRMdevel/RMsim/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="940" yWindow="1020" windowWidth="26620" windowHeight="11640"/>
+    <workbookView xWindow="360" yWindow="-105" windowWidth="29040" windowHeight="11640"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="segmentVolumesDensities" sheetId="1" r:id="rId1"/>
+    <sheet name="For export" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
-  <extLst>
+  <calcPr calcId="124519" concurrentCalc="0"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -27,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="46">
   <si>
     <t>Body segment</t>
   </si>
@@ -71,9 +67,6 @@
     <t>Foot soft tissues</t>
   </si>
   <si>
-    <t>lumped segment mass (from uCT)</t>
-  </si>
-  <si>
     <t>Body soft tissues</t>
   </si>
   <si>
@@ -141,13 +134,40 @@
   </si>
   <si>
     <t>mass for scaled model (g)</t>
+  </si>
+  <si>
+    <t>scaled masses (g)</t>
+  </si>
+  <si>
+    <t>lumped segment mass  (from uCT)</t>
+  </si>
+  <si>
+    <t>cylinder volume (cm3)</t>
+  </si>
+  <si>
+    <t>radius (cm)</t>
+  </si>
+  <si>
+    <t>radius (mm)</t>
+  </si>
+  <si>
+    <t>MOI xx</t>
+  </si>
+  <si>
+    <t>MOI yy</t>
+  </si>
+  <si>
+    <t>MOI zz</t>
+  </si>
+  <si>
+    <t>radius (m)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -252,7 +272,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -287,7 +307,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -464,45 +484,49 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:S18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="16.5" customWidth="1"/>
-    <col min="3" max="3" width="18.83203125" customWidth="1"/>
-    <col min="4" max="4" width="30.1640625" customWidth="1"/>
-    <col min="5" max="6" width="18.83203125" customWidth="1"/>
-    <col min="7" max="8" width="26.83203125" customWidth="1"/>
-    <col min="9" max="9" width="10" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" customWidth="1"/>
+    <col min="4" max="4" width="30.140625" customWidth="1"/>
+    <col min="5" max="6" width="18.85546875" customWidth="1"/>
+    <col min="7" max="9" width="26.85546875" customWidth="1"/>
+    <col min="10" max="10" width="10" customWidth="1"/>
+    <col min="13" max="13" width="13" customWidth="1"/>
+    <col min="14" max="14" width="12.140625" customWidth="1"/>
+    <col min="15" max="16" width="12" customWidth="1"/>
+    <col min="17" max="19" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19">
       <c r="E1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19">
       <c r="A2" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B2" s="1">
         <v>11.4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D2" s="2">
         <v>11.4</v>
@@ -512,7 +536,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -523,31 +547,55 @@
         <v>5</v>
       </c>
       <c r="D3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" t="s">
         <v>25</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I3" t="s">
+        <v>37</v>
+      </c>
+      <c r="J3" t="s">
         <v>26</v>
       </c>
-      <c r="F3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" t="s">
-        <v>28</v>
-      </c>
-      <c r="I3" t="s">
-        <v>27</v>
-      </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
+        <v>29</v>
+      </c>
+      <c r="L3" t="s">
         <v>30</v>
       </c>
-      <c r="K3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M3" t="s">
+        <v>39</v>
+      </c>
+      <c r="N3" t="s">
+        <v>40</v>
+      </c>
+      <c r="O3" t="s">
+        <v>41</v>
+      </c>
+      <c r="P3" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>42</v>
+      </c>
+      <c r="R3" t="s">
+        <v>43</v>
+      </c>
+      <c r="S3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -565,7 +613,7 @@
         <v>1.0997000000000001</v>
       </c>
       <c r="F4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G4">
         <v>7.1999999999999998E-3</v>
@@ -575,23 +623,55 @@
         <v>7.1999999999999998E-3</v>
       </c>
       <c r="I4">
+        <f>G4*$E$2*1000</f>
+        <v>7.2</v>
+      </c>
+      <c r="J4">
         <f>E4</f>
         <v>1.0997000000000001</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>1.9743900000000002E-2</v>
       </c>
-      <c r="K4">
-        <f>J4*($E$2^(1/3))</f>
+      <c r="L4">
+        <f>K4*($E$2^(1/3))</f>
         <v>1.9743900000000002E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M4">
+        <f t="shared" ref="M4:M9" si="0">I4/J4</f>
+        <v>6.5472401564062919</v>
+      </c>
+      <c r="N4">
+        <f>SQRT(M4/(3.141*L4*100))</f>
+        <v>1.0274925842859248</v>
+      </c>
+      <c r="O4">
+        <f>N4*10</f>
+        <v>10.274925842859249</v>
+      </c>
+      <c r="P4">
+        <f>O4/1000</f>
+        <v>1.0274925842859248E-2</v>
+      </c>
+      <c r="Q4">
+        <f>(1/12)*(H4*L4^2)+(1/4)*(H4*P4^2)</f>
+        <v>4.2392633426326229E-7</v>
+      </c>
+      <c r="R4">
+        <f>Q4</f>
+        <v>4.2392633426326229E-7</v>
+      </c>
+      <c r="S4">
+        <f>(1/2)*H4*P4^2</f>
+        <v>3.8006676387452462E-7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19">
       <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
         <v>15</v>
-      </c>
-      <c r="B5" t="s">
-        <v>16</v>
       </c>
       <c r="C5">
         <v>1.056</v>
@@ -601,24 +681,32 @@
         <v>0.95</v>
       </c>
       <c r="F5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G5">
         <v>1.2999999999999999E-3</v>
       </c>
       <c r="H5">
-        <f t="shared" ref="H5:H9" si="0">G5*$E$2</f>
+        <f t="shared" ref="H5:H9" si="1">G5*$E$2</f>
         <v>1.2999999999999999E-3</v>
       </c>
       <c r="I5">
+        <f t="shared" ref="I5:I9" si="2">G5*$E$2*1000</f>
+        <v>1.3</v>
+      </c>
+      <c r="J5">
         <f>E6</f>
         <v>1.0997000000000001</v>
       </c>
-      <c r="J5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="0"/>
+        <v>1.1821405837955805</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -636,33 +724,65 @@
         <v>1.0997000000000001</v>
       </c>
       <c r="F6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G6">
         <v>7.7612999999999998E-4</v>
       </c>
       <c r="H6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.7612999999999998E-4</v>
       </c>
       <c r="I6">
+        <f t="shared" si="2"/>
+        <v>0.77612999999999999</v>
+      </c>
+      <c r="J6">
         <f>E8</f>
         <v>1.0806231520223153</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>1.77912E-2</v>
       </c>
-      <c r="K6">
-        <f t="shared" ref="K5:K9" si="1">J6*($E$2^(1/3))</f>
+      <c r="L6">
+        <f t="shared" ref="L6:L9" si="3">K6*($E$2^(1/3))</f>
         <v>1.77912E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M6">
+        <f t="shared" si="0"/>
+        <v>0.71822447867003736</v>
+      </c>
+      <c r="N6">
+        <f t="shared" ref="N6:N9" si="4">SQRT(M6/(3.141*L6*100))</f>
+        <v>0.35850359270500043</v>
+      </c>
+      <c r="O6">
+        <f t="shared" ref="O6:O9" si="5">N6*10</f>
+        <v>3.5850359270500043</v>
+      </c>
+      <c r="P6">
+        <f t="shared" ref="P6:P9" si="6">O6/1000</f>
+        <v>3.5850359270500043E-3</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" ref="Q6:Q9" si="7">(1/12)*(H6*L6^2)+(1/4)*(H6*P6^2)</f>
+        <v>2.2965961271168462E-8</v>
+      </c>
+      <c r="R6">
+        <f t="shared" ref="R6:R9" si="8">Q6</f>
+        <v>2.2965961271168462E-8</v>
+      </c>
+      <c r="S6">
+        <f t="shared" ref="S6:S9" si="9">(1/2)*H6*P6^2</f>
+        <v>4.9875986594857276E-9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C7">
         <v>1.056</v>
@@ -672,28 +792,60 @@
         <v>0.95</v>
       </c>
       <c r="F7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G7">
         <v>3.6152999999999999E-4</v>
       </c>
       <c r="H7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.6152999999999999E-4</v>
       </c>
       <c r="I7">
+        <f t="shared" si="2"/>
+        <v>0.36152999999999996</v>
+      </c>
+      <c r="J7">
         <f>E10</f>
         <v>1.1300727394060728</v>
       </c>
-      <c r="J7">
-        <v>8.0277000000000005E-3</v>
-      </c>
       <c r="K7">
-        <f t="shared" si="1"/>
-        <v>8.0277000000000005E-3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+        <v>2.0467099999999998E-2</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="3"/>
+        <v>2.0467099999999998E-2</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="0"/>
+        <v>0.31991745964070212</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="4"/>
+        <v>0.22307805401213149</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="5"/>
+        <v>2.230780540121315</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="6"/>
+        <v>2.2307805401213148E-3</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" si="7"/>
+        <v>1.3070253330239283E-8</v>
+      </c>
+      <c r="R7">
+        <f t="shared" si="8"/>
+        <v>1.3070253330239283E-8</v>
+      </c>
+      <c r="S7">
+        <f t="shared" si="9"/>
+        <v>8.9955565936402089E-10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -712,28 +864,60 @@
         <v>1.0806231520223153</v>
       </c>
       <c r="F8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G8">
         <v>1.5557E-4</v>
       </c>
       <c r="H8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.5557E-4</v>
       </c>
       <c r="I8">
+        <f t="shared" si="2"/>
+        <v>0.15557000000000001</v>
+      </c>
+      <c r="J8">
         <f>E12</f>
         <v>1.154644041041831</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>8.0277000000000005E-3</v>
       </c>
-      <c r="K8">
-        <f t="shared" si="1"/>
+      <c r="L8">
+        <f t="shared" si="3"/>
         <v>8.0277000000000005E-3</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M8">
+        <f t="shared" si="0"/>
+        <v>0.13473416435738045</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="4"/>
+        <v>0.23115821449146384</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="5"/>
+        <v>2.3115821449146385</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="6"/>
+        <v>2.3115821449146384E-3</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="7"/>
+        <v>1.0432809843122492E-9</v>
+      </c>
+      <c r="R8">
+        <f t="shared" si="8"/>
+        <v>1.0432809843122492E-9</v>
+      </c>
+      <c r="S8">
+        <f t="shared" si="9"/>
+        <v>4.1563730340694859E-10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -748,28 +932,60 @@
         <v>0.97182705718270568</v>
       </c>
       <c r="F9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G9">
         <v>1.6291999999999999E-4</v>
       </c>
       <c r="H9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.6291999999999999E-4</v>
       </c>
       <c r="I9">
+        <f t="shared" si="2"/>
+        <v>0.16291999999999998</v>
+      </c>
+      <c r="J9">
         <f>E14</f>
         <v>1.2015483346872462</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>0.01</v>
       </c>
-      <c r="K9">
-        <f t="shared" si="1"/>
+      <c r="L9">
+        <f t="shared" si="3"/>
         <v>0.01</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M9">
+        <f t="shared" si="0"/>
+        <v>0.13559171553627661</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="4"/>
+        <v>0.20776988987018494</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="5"/>
+        <v>2.0776988987018492</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="6"/>
+        <v>2.0776988987018493E-3</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" si="7"/>
+        <v>1.5334912630943186E-9</v>
+      </c>
+      <c r="R9">
+        <f t="shared" si="8"/>
+        <v>1.5334912630943186E-9</v>
+      </c>
+      <c r="S9">
+        <f t="shared" si="9"/>
+        <v>3.5164919285530379E-10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -788,7 +1004,7 @@
         <v>1.1300727394060728</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:19">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -803,7 +1019,7 @@
         <v>0.9152485819152486</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:19">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -823,7 +1039,7 @@
         <v>1.154644041041831</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:19">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -838,7 +1054,7 @@
         <v>0.88713496448303075</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:19">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -858,7 +1074,7 @@
         <v>1.2015483346872462</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:19">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -873,39 +1089,39 @@
         <v>0.8334687246141349</v>
       </c>
       <c r="G15" t="s">
+        <v>31</v>
+      </c>
+      <c r="I15" t="s">
         <v>32</v>
       </c>
-      <c r="H15" t="s">
+      <c r="J15" t="s">
         <v>33</v>
       </c>
-      <c r="I15" t="s">
+      <c r="K15" t="s">
         <v>34</v>
       </c>
-      <c r="J15" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:19">
       <c r="G16">
         <v>27</v>
       </c>
-      <c r="H16">
+      <c r="I16">
         <v>10</v>
       </c>
-      <c r="I16">
+      <c r="J16">
         <f>G16^(1/3)</f>
         <v>2.9999999999999996</v>
       </c>
-      <c r="J16">
-        <f>I16*(H16/G16)^(1/3)</f>
+      <c r="K16">
+        <f>J16*(I16/G16)^(1/3)</f>
         <v>2.1544346900318834</v>
       </c>
-      <c r="K16">
-        <f>J16^3</f>
+      <c r="L16">
+        <f>K16^3</f>
         <v>9.9999999999999947</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -919,4 +1135,16 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>